<commit_message>
Add some sorting algs on C, benchmark more precise, add results into table
</commit_message>
<xml_diff>
--- a/results/table.xlsx
+++ b/results/table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elect\go\src\sortResearch\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8828DD20-583E-4805-BA12-817CE3CAB94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06522DE2-6197-419E-A1E2-006F056A4484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{124C95DA-02F8-4AC3-976E-42FE8A7572FA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Go</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Merge Sort</t>
-  </si>
-  <si>
-    <t>Merge Parallel Sort</t>
   </si>
   <si>
     <t>Quick Sort</t>
@@ -106,7 +103,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,6 +119,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -190,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -199,14 +202,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -224,12 +225,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -548,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D11F4383-1679-44EF-B74F-D21FE1B13C0C}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,74 +564,74 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
-      <c r="C1" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
+      <c r="C1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" s="13"/>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15" t="s">
+      <c r="J2" s="8"/>
+      <c r="K2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="15"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="14"/>
       <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="I3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="K3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -644,15 +639,18 @@
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="6">
         <v>10000</v>
       </c>
       <c r="D4" s="4">
-        <f>80378879*(10^(-6))</f>
-        <v>80.378878999999998</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="E4" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F4" s="2">
+        <v>61</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -663,15 +661,18 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="10"/>
-      <c r="C5" s="2">
+      <c r="C5" s="6">
         <v>25000</v>
       </c>
       <c r="D5" s="4">
-        <f>754053500*(10^(-6))</f>
-        <v>754.05349999999999</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+        <v>745</v>
+      </c>
+      <c r="E5" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F5" s="2">
+        <v>535</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -682,15 +683,18 @@
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="10"/>
-      <c r="C6" s="2">
+      <c r="C6" s="6">
         <v>50000</v>
       </c>
       <c r="D6" s="4">
-        <f>3535001900*(10^(-6))</f>
-        <v>3535.0018999999998</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+        <v>3543</v>
+      </c>
+      <c r="E6" s="6">
+        <v>50000</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2462</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -701,15 +705,18 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="2">
+      <c r="C7" s="6">
         <v>100000</v>
       </c>
       <c r="D7" s="4">
-        <f>14775713500*(10^(-6))</f>
-        <v>14775.7135</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+        <v>14712</v>
+      </c>
+      <c r="E7" s="6">
+        <v>100000</v>
+      </c>
+      <c r="F7" s="2">
+        <v>10290</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -720,15 +727,18 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="2">
+      <c r="C8" s="6">
         <v>150000</v>
       </c>
       <c r="D8" s="4">
-        <f>33688304100*(10^(-6))</f>
-        <v>33688.304100000001</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+        <v>33101</v>
+      </c>
+      <c r="E8" s="6">
+        <v>150000</v>
+      </c>
+      <c r="F8" s="2">
+        <v>25662</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -738,15 +748,18 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" s="10"/>
-      <c r="C9" s="2">
+      <c r="C9" s="6">
         <v>300000</v>
       </c>
       <c r="D9" s="4">
-        <f>133938048600*(10^(-6))</f>
-        <v>133938.04859999998</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+        <v>132438</v>
+      </c>
+      <c r="E9" s="6">
+        <v>300000</v>
+      </c>
+      <c r="F9" s="2">
+        <v>103491</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -756,15 +769,18 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" s="11"/>
-      <c r="C10" s="2">
+      <c r="C10" s="6">
         <v>500000</v>
       </c>
       <c r="D10" s="4">
-        <f>372575739700*(10^(-6))</f>
-        <v>372575.73969999998</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+        <v>367257</v>
+      </c>
+      <c r="E10" s="6">
+        <v>500000</v>
+      </c>
+      <c r="F10" s="2">
+        <v>288911</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -776,15 +792,18 @@
       <c r="B11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="6">
         <v>10000</v>
       </c>
       <c r="D11" s="4">
-        <f>39813714*(10^(-6))</f>
-        <v>39.813713999999997</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="E11" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F11" s="2">
+        <v>39</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -794,15 +813,18 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" s="10"/>
-      <c r="C12" s="2">
+      <c r="C12" s="6">
         <v>25000</v>
       </c>
       <c r="D12" s="4">
-        <f>244032020*(10^(-6))</f>
-        <v>244.03201999999999</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+        <v>240</v>
+      </c>
+      <c r="E12" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F12" s="2">
+        <v>237</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -812,15 +834,18 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" s="10"/>
-      <c r="C13" s="2">
+      <c r="C13" s="6">
         <v>50000</v>
       </c>
       <c r="D13" s="4">
-        <f>975045600*(10^(-6))</f>
-        <v>975.04559999999992</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+        <v>952</v>
+      </c>
+      <c r="E13" s="6">
+        <v>50000</v>
+      </c>
+      <c r="F13" s="2">
+        <v>946</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -830,15 +855,18 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
-      <c r="C14" s="2">
+      <c r="C14" s="6">
         <v>100000</v>
       </c>
       <c r="D14" s="4">
-        <f>3850774300*(10^(-6))</f>
-        <v>3850.7743</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+        <v>3797</v>
+      </c>
+      <c r="E14" s="6">
+        <v>100000</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3776</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -848,15 +876,18 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" s="10"/>
-      <c r="C15" s="2">
+      <c r="C15" s="6">
         <v>150000</v>
       </c>
       <c r="D15" s="4">
-        <f>8716052400*(10^(-6))</f>
-        <v>8716.0524000000005</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+        <v>8539</v>
+      </c>
+      <c r="E15" s="6">
+        <v>150000</v>
+      </c>
+      <c r="F15" s="2">
+        <v>8494</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -866,15 +897,18 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" s="10"/>
-      <c r="C16" s="2">
+      <c r="C16" s="6">
         <v>300000</v>
       </c>
       <c r="D16" s="4">
-        <f>35770580900*(10^(-6))</f>
-        <v>35770.580900000001</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+        <v>34159</v>
+      </c>
+      <c r="E16" s="6">
+        <v>300000</v>
+      </c>
+      <c r="F16" s="2">
+        <v>33964</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -884,15 +918,18 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="11"/>
-      <c r="C17" s="2">
+      <c r="C17" s="6">
         <v>500000</v>
       </c>
       <c r="D17" s="4">
-        <f>102016309900*(10^(-6))</f>
-        <v>102016.30989999999</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+        <v>95020</v>
+      </c>
+      <c r="E17" s="6">
+        <v>500000</v>
+      </c>
+      <c r="F17" s="2">
+        <v>94355</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -904,15 +941,18 @@
       <c r="B18" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="6">
         <v>10000</v>
       </c>
       <c r="D18" s="4">
-        <f>45586654*(10^(-6))</f>
-        <v>45.586653999999996</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="E18" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F18" s="2">
+        <v>46</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -922,15 +962,18 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="10"/>
-      <c r="C19" s="2">
+      <c r="C19" s="6">
         <v>25000</v>
       </c>
       <c r="D19" s="4">
-        <f>280996525*(10^(-6))</f>
-        <v>280.99652499999996</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+        <v>277</v>
+      </c>
+      <c r="E19" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F19" s="2">
+        <v>277</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -940,15 +983,18 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="10"/>
-      <c r="C20" s="2">
+      <c r="C20" s="6">
         <v>50000</v>
       </c>
       <c r="D20" s="4">
-        <f>1136717300*(10^(-6))</f>
-        <v>1136.7173</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+        <v>1116</v>
+      </c>
+      <c r="E20" s="6">
+        <v>50000</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1121</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -958,15 +1004,18 @@
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="10"/>
-      <c r="C21" s="2">
+      <c r="C21" s="6">
         <v>100000</v>
       </c>
       <c r="D21" s="4">
-        <f>4511646700*(10^(-6))</f>
-        <v>4511.6467000000002</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+        <v>4449</v>
+      </c>
+      <c r="E21" s="6">
+        <v>100000</v>
+      </c>
+      <c r="F21" s="2">
+        <v>4474</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -976,15 +1025,18 @@
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="10"/>
-      <c r="C22" s="2">
+      <c r="C22" s="6">
         <v>150000</v>
       </c>
       <c r="D22" s="4">
-        <f>10087775000*(10^(-6))</f>
-        <v>10087.775</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+        <v>9964</v>
+      </c>
+      <c r="E22" s="6">
+        <v>150000</v>
+      </c>
+      <c r="F22" s="2">
+        <v>10029</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -994,15 +1046,18 @@
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="10"/>
-      <c r="C23" s="2">
+      <c r="C23" s="6">
         <v>300000</v>
       </c>
       <c r="D23" s="4">
-        <f>41367650800*(10^(-6))</f>
-        <v>41367.650799999996</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+        <v>39985</v>
+      </c>
+      <c r="E23" s="6">
+        <v>300000</v>
+      </c>
+      <c r="F23" s="2">
+        <v>40191</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1012,15 +1067,18 @@
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="11"/>
-      <c r="C24" s="2">
+      <c r="C24" s="6">
         <v>500000</v>
       </c>
       <c r="D24" s="4">
-        <f>112281387100*(10^(-6))</f>
-        <v>112281.38709999999</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+        <v>111014</v>
+      </c>
+      <c r="E24" s="6">
+        <v>500000</v>
+      </c>
+      <c r="F24" s="2">
+        <v>111593</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1032,15 +1090,19 @@
       <c r="B25" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="6">
         <v>10000</v>
       </c>
       <c r="D25" s="4">
         <f>1962311*(10^(-6))</f>
         <v>1.9623109999999999</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="E25" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1050,15 +1112,19 @@
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" s="10"/>
-      <c r="C26" s="2">
+      <c r="C26" s="6">
         <v>25000</v>
       </c>
       <c r="D26" s="4">
         <f>5046928*(10^(-6))</f>
         <v>5.0469279999999994</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="E26" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F26" s="2">
+        <v>3</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1068,15 +1134,19 @@
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="10"/>
-      <c r="C27" s="2">
+      <c r="C27" s="6">
         <v>50000</v>
       </c>
       <c r="D27" s="4">
         <f>10367642*(10^(-6))</f>
         <v>10.367642</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="E27" s="6">
+        <v>50000</v>
+      </c>
+      <c r="F27" s="2">
+        <v>7</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -1086,15 +1156,18 @@
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="10"/>
-      <c r="C28" s="2">
+      <c r="C28" s="6">
         <v>100000</v>
       </c>
       <c r="D28" s="4">
-        <f>21514532*(10^(-6))</f>
-        <v>21.514531999999999</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="E28" s="6">
+        <v>100000</v>
+      </c>
+      <c r="F28" s="2">
+        <v>14</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -1104,15 +1177,19 @@
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" s="10"/>
-      <c r="C29" s="2">
+      <c r="C29" s="6">
         <v>150000</v>
       </c>
       <c r="D29" s="4">
         <f>32453025*(10^(-6))</f>
         <v>32.453024999999997</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="E29" s="6">
+        <v>150000</v>
+      </c>
+      <c r="F29" s="2">
+        <v>22</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -1122,15 +1199,18 @@
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="10"/>
-      <c r="C30" s="2">
+      <c r="C30" s="6">
         <v>300000</v>
       </c>
       <c r="D30" s="4">
-        <f>67414117*(10^(-6))</f>
-        <v>67.41411699999999</v>
-      </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="E30" s="6">
+        <v>300000</v>
+      </c>
+      <c r="F30" s="2">
+        <v>45</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -1140,15 +1220,18 @@
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="11"/>
-      <c r="C31" s="2">
+      <c r="C31" s="6">
         <v>500000</v>
       </c>
       <c r="D31" s="4">
-        <f>113206756*(10^(-6))</f>
-        <v>113.206756</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+        <v>111</v>
+      </c>
+      <c r="E31" s="6">
+        <v>500000</v>
+      </c>
+      <c r="F31" s="2">
+        <v>77</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -1157,18 +1240,22 @@
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="6">
         <v>10000</v>
       </c>
       <c r="D32" s="4">
-        <f>1717754*(10^(-6))</f>
-        <v>1.717754</v>
-      </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+        <f>1383828*(10^(-6))</f>
+        <v>1.3838279999999998</v>
+      </c>
+      <c r="E32" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -1177,16 +1264,20 @@
       <c r="L32" s="2"/>
     </row>
     <row r="33" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="7"/>
-      <c r="C33" s="2">
+      <c r="B33" s="10"/>
+      <c r="C33" s="6">
         <v>25000</v>
       </c>
       <c r="D33" s="4">
-        <f>4457219*(10^(-6))</f>
-        <v>4.4572189999999994</v>
-      </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+        <f>3632421*(10^(-6))</f>
+        <v>3.6324209999999999</v>
+      </c>
+      <c r="E33" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -1195,16 +1286,20 @@
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="7"/>
-      <c r="C34" s="2">
+      <c r="B34" s="10"/>
+      <c r="C34" s="6">
         <v>50000</v>
       </c>
       <c r="D34" s="4">
-        <f>8401827*(10^(-6))</f>
-        <v>8.401826999999999</v>
-      </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+        <f>7332698*(10^(-6))</f>
+        <v>7.3326979999999997</v>
+      </c>
+      <c r="E34" s="6">
+        <v>50000</v>
+      </c>
+      <c r="F34" s="2">
+        <v>3</v>
+      </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -1213,16 +1308,20 @@
       <c r="L34" s="2"/>
     </row>
     <row r="35" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="7"/>
-      <c r="C35" s="2">
+      <c r="B35" s="10"/>
+      <c r="C35" s="6">
         <v>100000</v>
       </c>
       <c r="D35" s="4">
-        <f>16326157*(10^(-6))</f>
-        <v>16.326156999999998</v>
-      </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+        <f>14954158*(10^(-6))</f>
+        <v>14.954158</v>
+      </c>
+      <c r="E35" s="6">
+        <v>100000</v>
+      </c>
+      <c r="F35" s="2">
+        <v>6</v>
+      </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -1231,16 +1330,19 @@
       <c r="L35" s="2"/>
     </row>
     <row r="36" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="7"/>
-      <c r="C36" s="2">
+      <c r="B36" s="10"/>
+      <c r="C36" s="6">
         <v>150000</v>
       </c>
       <c r="D36" s="4">
-        <f>24181863*(10^(-6))</f>
-        <v>24.181863</v>
-      </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="E36" s="6">
+        <v>150000</v>
+      </c>
+      <c r="F36" s="2">
+        <v>9</v>
+      </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -1249,16 +1351,19 @@
       <c r="L36" s="2"/>
     </row>
     <row r="37" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="7"/>
-      <c r="C37" s="2">
+      <c r="B37" s="10"/>
+      <c r="C37" s="6">
         <v>300000</v>
       </c>
       <c r="D37" s="4">
-        <f>49644882*(10^(-6))</f>
-        <v>49.644881999999996</v>
-      </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="E37" s="6">
+        <v>300000</v>
+      </c>
+      <c r="F37" s="2">
+        <v>18</v>
+      </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -1267,16 +1372,19 @@
       <c r="L37" s="2"/>
     </row>
     <row r="38" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="8"/>
-      <c r="C38" s="2">
+      <c r="B38" s="11"/>
+      <c r="C38" s="6">
         <v>500000</v>
       </c>
       <c r="D38" s="4">
-        <f>83354307*(10^(-6))</f>
-        <v>83.354306999999991</v>
-      </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="E38" s="6">
+        <v>500000</v>
+      </c>
+      <c r="F38" s="2">
+        <v>33</v>
+      </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
@@ -1284,152 +1392,30 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="2">
-        <v>10000</v>
-      </c>
-      <c r="D39" s="4">
-        <f>1383828*(10^(-6))</f>
-        <v>1.3838279999999998</v>
-      </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-    </row>
-    <row r="40" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="10"/>
-      <c r="C40" s="2">
-        <v>25000</v>
-      </c>
-      <c r="D40" s="4">
-        <f>3632421*(10^(-6))</f>
-        <v>3.6324209999999999</v>
-      </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-    </row>
-    <row r="41" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="10"/>
-      <c r="C41" s="2">
-        <v>50000</v>
-      </c>
-      <c r="D41" s="4">
-        <f>7332698*(10^(-6))</f>
-        <v>7.3326979999999997</v>
-      </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-    </row>
-    <row r="42" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="10"/>
-      <c r="C42" s="2">
-        <v>100000</v>
-      </c>
-      <c r="D42" s="4">
-        <f>14954158*(10^(-6))</f>
-        <v>14.954158</v>
-      </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-    </row>
-    <row r="43" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="10"/>
-      <c r="C43" s="2">
-        <v>150000</v>
-      </c>
-      <c r="D43" s="4">
-        <f>22727572*(10^(-6))</f>
-        <v>22.727571999999999</v>
-      </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-    </row>
-    <row r="44" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="10"/>
-      <c r="C44" s="2">
-        <v>300000</v>
-      </c>
-      <c r="D44" s="4">
-        <f>46248600*(10^(-6))</f>
-        <v>46.248599999999996</v>
-      </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-    </row>
-    <row r="45" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="11"/>
-      <c r="C45" s="2">
-        <v>500000</v>
-      </c>
-      <c r="D45" s="4">
-        <f>78952021*(10^(-6))</f>
-        <v>78.952021000000002</v>
-      </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-    </row>
+    <row r="39" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B47" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="12">
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="B25:B31"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="B39:B45"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="B25:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix c files, add cpp folder
</commit_message>
<xml_diff>
--- a/results/table.xlsx
+++ b/results/table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elect\go\src\sortResearch\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06522DE2-6197-419E-A1E2-006F056A4484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C4427B-2DC4-4F5B-B507-083E0F41FB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{124C95DA-02F8-4AC3-976E-42FE8A7572FA}"/>
   </bookViews>
@@ -203,12 +203,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -225,6 +219,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D11F4383-1679-44EF-B74F-D21FE1B13C0C}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,46 +563,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="12"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="13"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="8"/>
+      <c r="L2" s="14"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="14"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
@@ -636,7 +636,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="6">
@@ -660,7 +660,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="10"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="6">
         <v>25000</v>
       </c>
@@ -682,7 +682,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="10"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="6">
         <v>50000</v>
       </c>
@@ -704,7 +704,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="10"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="6">
         <v>100000</v>
       </c>
@@ -726,7 +726,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="10"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="6">
         <v>150000</v>
       </c>
@@ -747,7 +747,7 @@
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="10"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="6">
         <v>300000</v>
       </c>
@@ -768,7 +768,7 @@
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="11"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="6">
         <v>500000</v>
       </c>
@@ -789,7 +789,7 @@
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="6">
@@ -812,7 +812,7 @@
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="10"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="6">
         <v>25000</v>
       </c>
@@ -833,7 +833,7 @@
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="10"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="6">
         <v>50000</v>
       </c>
@@ -854,7 +854,7 @@
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="10"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="6">
         <v>100000</v>
       </c>
@@ -875,7 +875,7 @@
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="10"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="6">
         <v>150000</v>
       </c>
@@ -896,7 +896,7 @@
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="10"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="6">
         <v>300000</v>
       </c>
@@ -917,7 +917,7 @@
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="11"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="6">
         <v>500000</v>
       </c>
@@ -938,7 +938,7 @@
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="6">
@@ -961,7 +961,7 @@
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="6">
         <v>25000</v>
       </c>
@@ -982,7 +982,7 @@
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B20" s="10"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="6">
         <v>50000</v>
       </c>
@@ -1003,7 +1003,7 @@
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B21" s="10"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="6">
         <v>100000</v>
       </c>
@@ -1024,7 +1024,7 @@
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="10"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="6">
         <v>150000</v>
       </c>
@@ -1045,7 +1045,7 @@
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B23" s="10"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="6">
         <v>300000</v>
       </c>
@@ -1066,7 +1066,7 @@
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="11"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="6">
         <v>500000</v>
       </c>
@@ -1087,7 +1087,7 @@
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="6">
@@ -1111,7 +1111,7 @@
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B26" s="10"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="6">
         <v>25000</v>
       </c>
@@ -1133,7 +1133,7 @@
       <c r="L26" s="2"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="10"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="6">
         <v>50000</v>
       </c>
@@ -1155,7 +1155,7 @@
       <c r="L27" s="2"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B28" s="10"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="6">
         <v>100000</v>
       </c>
@@ -1176,7 +1176,7 @@
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B29" s="10"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="6">
         <v>150000</v>
       </c>
@@ -1198,7 +1198,7 @@
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B30" s="10"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="6">
         <v>300000</v>
       </c>
@@ -1219,7 +1219,7 @@
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B31" s="11"/>
+      <c r="B31" s="9"/>
       <c r="C31" s="6">
         <v>500000</v>
       </c>
@@ -1240,7 +1240,7 @@
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="6">
@@ -1264,7 +1264,7 @@
       <c r="L32" s="2"/>
     </row>
     <row r="33" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="10"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="6">
         <v>25000</v>
       </c>
@@ -1286,7 +1286,7 @@
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="10"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="6">
         <v>50000</v>
       </c>
@@ -1308,7 +1308,7 @@
       <c r="L34" s="2"/>
     </row>
     <row r="35" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="10"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="6">
         <v>100000</v>
       </c>
@@ -1330,7 +1330,7 @@
       <c r="L35" s="2"/>
     </row>
     <row r="36" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="10"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="6">
         <v>150000</v>
       </c>
@@ -1351,7 +1351,7 @@
       <c r="L36" s="2"/>
     </row>
     <row r="37" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="10"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="6">
         <v>300000</v>
       </c>
@@ -1372,7 +1372,7 @@
       <c r="L37" s="2"/>
     </row>
     <row r="38" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="11"/>
+      <c r="B38" s="9"/>
       <c r="C38" s="6">
         <v>500000</v>
       </c>
@@ -1404,18 +1404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="B32:B38"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="B4:B10"/>
     <mergeCell ref="B11:B17"/>
     <mergeCell ref="B18:B24"/>
     <mergeCell ref="B25:B31"/>
-    <mergeCell ref="C1:L1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>